<commit_message>
Worked: draft for testing super convergence
</commit_message>
<xml_diff>
--- a/working/Perturb/log/tables/table2.xlsx
+++ b/working/Perturb/log/tables/table2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab_codes\FEM\FiniteElemntMethod\working\Perturb\log\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FFE11F-D200-456C-BEC8-0825AF60DFA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F83F5C-56A6-4F94-9C42-87B503338FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="-108" windowWidth="22128" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -170,6 +170,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -453,7 +454,7 @@
   <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,6 +1274,7 @@
         <f t="shared" si="3"/>
         <v>0.9987456115856761</v>
       </c>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">

</xml_diff>